<commit_message>
modified:   Pivot Tables & Pivot Charts/241 - Summarise data with PivotTables.xlsx modified:   Pivot Tables & Pivot Charts/242 - Customise PivotTables.xlsx modified:   Pivot Tables & Pivot Charts/243 - Group and sort pivot data.xlsx modified:   Pivot Tables & Pivot Charts/244 - Filter pivot data.xlsx modified:   Pivot Tables & Pivot Charts/245 - Performing calculations in pivots.xlsx modified:   Pivot Tables & Pivot Charts/246 - PivotCharts and other visualisations.xlsx new file:   Pivot Tables & Pivot Charts/C2W4-Practice-Challenge-soln.xlsx new file:   Pivot Tables & Pivot Charts/C2W4-Practice-Challenge.xlsx modified:   Pivot Tables & Pivot Charts/Demo.xlsx
</commit_message>
<xml_diff>
--- a/Pivot Tables & Pivot Charts/Demo.xlsx
+++ b/Pivot Tables & Pivot Charts/Demo.xlsx
@@ -1,30 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mq20161829\Documents\Data Wrangling MOOC\Course2\Week4\Workbooks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data-Visualizations-in-Excel\Pivot Tables &amp; Pivot Charts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8F96B51-225E-4968-8E04-4B3A5CAA27F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF994219-E711-4A49-991D-52BCA1F90747}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23136" yWindow="-96" windowWidth="23232" windowHeight="13152" xr2:uid="{67AA3378-DE12-456E-B786-995F0D74C9A0}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="22080" windowHeight="13176" activeTab="2" xr2:uid="{67AA3378-DE12-456E-B786-995F0D74C9A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="6" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlcn.WorksheetConnection_Demo.xlsxTable11" hidden="1">Table1[]</definedName>
+  </definedNames>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="183" r:id="rId4"/>
-    <pivotCache cacheId="238" r:id="rId5"/>
+    <pivotCache cacheId="8" r:id="rId4"/>
+    <pivotCache cacheId="12" r:id="rId5"/>
+    <pivotCache cacheId="10" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{FCE2AD5D-F65C-4FA6-A056-5C36A1767C68}">
+      <x15:dataModel>
+        <x15:modelTables>
+          <x15:modelTable id="Table1" name="Table1" connection="WorksheetConnection_Demo.xlsx!Table1"/>
+        </x15:modelTables>
+      </x15:dataModel>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -38,8 +49,31 @@
 </workbook>
 </file>
 
+<file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{45200E31-D657-4B56-8E62-951C8264259F}" keepAlive="1" name="ThisWorkbookDataModel" description="Data Model" type="5" refreshedVersion="8" minRefreshableVersion="5" background="1">
+    <dbPr connection="Data Model Connection" command="Model" commandType="1"/>
+    <olapPr sendLocale="1" rowDrillCount="1000"/>
+    <extLst>
+      <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
+        <x15:connection id="" model="1"/>
+      </ext>
+    </extLst>
+  </connection>
+  <connection id="2" xr16:uid="{29D1CA23-BB91-4AB2-BEB4-93529D6669F7}" name="WorksheetConnection_Demo.xlsx!Table1" type="102" refreshedVersion="8" minRefreshableVersion="5">
+    <extLst>
+      <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
+        <x15:connection id="Table1" autoDelete="1">
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_Demo.xlsxTable11"/>
+        </x15:connection>
+      </ext>
+    </extLst>
+  </connection>
+</connections>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="49">
   <si>
     <t>May</t>
   </si>
@@ -150,6 +184,42 @@
   </si>
   <si>
     <t>Total Cost</t>
+  </si>
+  <si>
+    <t>January</t>
+  </si>
+  <si>
+    <t>February</t>
+  </si>
+  <si>
+    <t>March</t>
+  </si>
+  <si>
+    <t>April</t>
+  </si>
+  <si>
+    <t>June</t>
+  </si>
+  <si>
+    <t>July</t>
+  </si>
+  <si>
+    <t>August</t>
+  </si>
+  <si>
+    <t>September</t>
+  </si>
+  <si>
+    <t>October</t>
+  </si>
+  <si>
+    <t>November</t>
+  </si>
+  <si>
+    <t>December</t>
+  </si>
+  <si>
+    <t>Sum of Cost</t>
   </si>
 </sst>
 </file>
@@ -157,8 +227,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="0;;"/>
+    <numFmt numFmtId="164" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="0;;"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -201,23 +271,38 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="6">
+    <dxf>
+      <alignment horizontal="right"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -261,7 +346,7 @@
         <s v="Anne"/>
       </sharedItems>
     </cacheField>
-    <cacheField name="Sales" numFmtId="44">
+    <cacheField name="Sales" numFmtId="164">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2568" maxValue="59112"/>
     </cacheField>
   </cacheFields>
@@ -278,7 +363,7 @@
   <cacheSource type="worksheet">
     <worksheetSource name="tblSales"/>
   </cacheSource>
-  <cacheFields count="4">
+  <cacheFields count="5">
     <cacheField name="Category" numFmtId="0">
       <sharedItems count="3">
         <s v="A"/>
@@ -321,6 +406,7 @@
     <cacheField name="Quantity" numFmtId="0">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2" maxValue="5"/>
     </cacheField>
+    <cacheField name="Cost" numFmtId="0" formula="Price*Quantity" databaseField="0"/>
   </cacheFields>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
@@ -330,6 +416,76 @@
 </pivotCacheDefinition>
 </file>
 
+<file path=xl/pivotCache/pivotCacheDefinition3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshedBy="Anoban" refreshedDate="44895.149109143516" backgroundQuery="1" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{835C90BB-9161-4AF3-96DF-E952EFE2D6DC}">
+  <cacheSource type="external" connectionId="1"/>
+  <cacheFields count="3">
+    <cacheField name="[Table1].[Day].[Day]" caption="Day" numFmtId="0" level="1">
+      <sharedItems count="7">
+        <s v="Friday"/>
+        <s v="Monday"/>
+        <s v="Saturday"/>
+        <s v="Sunday"/>
+        <s v="Thursday"/>
+        <s v="Tuesday"/>
+        <s v="Wednesday"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="[Measures].[Sum of Sales]" caption="Sum of Sales" numFmtId="0" hierarchy="5" level="32767"/>
+    <cacheField name="[Table1].[SalesPerson].[SalesPerson]" caption="SalesPerson" numFmtId="0" hierarchy="1" level="1">
+      <sharedItems count="3">
+        <s v="Anne"/>
+        <s v="May"/>
+        <s v="Sally"/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+  <cacheHierarchies count="6">
+    <cacheHierarchy uniqueName="[Table1].[Day]" caption="Day" attribute="1" defaultMemberUniqueName="[Table1].[Day].[All]" allUniqueName="[Table1].[Day].[All]" dimensionUniqueName="[Table1]" displayFolder="" count="2" memberValueDatatype="130" unbalanced="0">
+      <fieldsUsage count="2">
+        <fieldUsage x="-1"/>
+        <fieldUsage x="0"/>
+      </fieldsUsage>
+    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[Table1].[SalesPerson]" caption="SalesPerson" attribute="1" defaultMemberUniqueName="[Table1].[SalesPerson].[All]" allUniqueName="[Table1].[SalesPerson].[All]" dimensionUniqueName="[Table1]" displayFolder="" count="2" memberValueDatatype="130" unbalanced="0">
+      <fieldsUsage count="2">
+        <fieldUsage x="-1"/>
+        <fieldUsage x="2"/>
+      </fieldsUsage>
+    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[Table1].[Sales]" caption="Sales" attribute="1" defaultMemberUniqueName="[Table1].[Sales].[All]" allUniqueName="[Table1].[Sales].[All]" dimensionUniqueName="[Table1]" displayFolder="" count="0" memberValueDatatype="20" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Measures].[__XL_Count Table1]" caption="__XL_Count Table1" measure="1" displayFolder="" measureGroup="Table1" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[__No measures defined]" caption="__No measures defined" measure="1" displayFolder="" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[Sum of Sales]" caption="Sum of Sales" measure="1" displayFolder="" measureGroup="Table1" count="0" oneField="1" hidden="1">
+      <fieldsUsage count="1">
+        <fieldUsage x="1"/>
+      </fieldsUsage>
+      <extLst>
+        <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{B97F6D7D-B522-45F9-BDA1-12C45D357490}">
+          <x15:cacheHierarchy aggregatedColumn="2"/>
+        </ext>
+      </extLst>
+    </cacheHierarchy>
+  </cacheHierarchies>
+  <kpis count="0"/>
+  <dimensions count="2">
+    <dimension measure="1" name="Measures" uniqueName="[Measures]" caption="Measures"/>
+    <dimension name="Table1" uniqueName="[Table1]" caption="Table1"/>
+  </dimensions>
+  <measureGroups count="1">
+    <measureGroup name="Table1" caption="Table1"/>
+  </measureGroups>
+  <maps count="1">
+    <map measureGroup="0" dimension="1"/>
+  </maps>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition supportSubqueryNonVisual="1" supportSubqueryCalcMem="1" supportAddCalcMems="1"/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="21">
   <r>
@@ -518,9 +674,9 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{256C7C3C-0F44-4AD2-AB18-5AB69FD84D3D}" name="PivotTable23" cacheId="238" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="H2:I15" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="4">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{256C7C3C-0F44-4AD2-AB18-5AB69FD84D3D}" name="PivotTable23" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="H2:J15" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="5">
     <pivotField showAll="0"/>
     <pivotField axis="axisRow" showAll="0">
       <items count="26">
@@ -554,6 +710,7 @@
     </pivotField>
     <pivotField showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
   </pivotFields>
   <rowFields count="1">
     <field x="1"/>
@@ -599,11 +756,20 @@
       <x/>
     </i>
   </rowItems>
-  <colItems count="1">
-    <i/>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
   </colItems>
-  <dataFields count="1">
+  <dataFields count="2">
     <dataField name="Sum of Quantity" fld="3" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Cost" fld="4" baseField="0" baseItem="0"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -618,7 +784,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{12B1A451-1274-400B-A92D-884B8931CAFC}" name="PivotTable3" cacheId="183" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{12B1A451-1274-400B-A92D-884B8931CAFC}" name="PivotTable3" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:A4" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
   <pivotFields count="3">
     <pivotField showAll="0">
@@ -641,7 +807,7 @@
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField dataField="1" numFmtId="44" showAll="0"/>
+    <pivotField dataField="1" numFmtId="164" showAll="0"/>
   </pivotFields>
   <rowItems count="1">
     <i/>
@@ -664,6 +830,95 @@
 </pivotTableDefinition>
 </file>
 
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0E75B9DB-DC70-44DB-B1D2-550A95EED783}" name="PivotTable5" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="F1:G5" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="3">
+    <pivotField allDrilled="1" subtotalTop="0" showAll="0" sortType="ascending" defaultSubtotal="0" defaultAttributeDrillState="1">
+      <items count="7">
+        <item x="3"/>
+        <item x="1"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="4"/>
+        <item x="0"/>
+        <item x="2"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" subtotalTop="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField axis="axisRow" allDrilled="1" subtotalTop="0" showAll="0" defaultSubtotal="0" defaultAttributeDrillState="1">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item x="2"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="2"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Sales" fld="1" baseField="0" baseItem="0"/>
+  </dataFields>
+  <formats count="4">
+    <format dxfId="3">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="2">
+      <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="1">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="0">
+      <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
+    </format>
+  </formats>
+  <pivotHierarchies count="6">
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+  </pivotHierarchies>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <rowHierarchiesUsage count="1">
+    <rowHierarchyUsage hierarchyUsage="1"/>
+  </rowHierarchiesUsage>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" calculatedMembersInFilters="1" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{E67621CE-5B39-4880-91FE-76760E9C1902}">
+      <x15:pivotTableUISettings sourceDataName="WorksheetConnection_Demo.xlsx!Table1">
+        <x15:activeTabTopLevelEntity name="[Table1]"/>
+      </x15:pivotTableUISettings>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16 EnabledSubtotalsDefault="0" SubtotalsOnTopDefault="0"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2072DAE7-B3BE-4CBE-BF21-D3F4EF193FB2}" name="tblSales" displayName="tblSales" ref="A2:D15" totalsRowCount="1">
   <autoFilter ref="A2:D14" xr:uid="{630D84E0-E091-415F-91B0-E22B93557B87}"/>
@@ -671,7 +926,7 @@
     <tableColumn id="1" xr3:uid="{24F201BC-6B22-41ED-A0AA-804147DDDD5E}" name="Category"/>
     <tableColumn id="2" xr3:uid="{B2539B1A-DC56-48C9-B75A-622CBA12A5DF}" name="Product"/>
     <tableColumn id="3" xr3:uid="{B0B44DF2-95E5-438F-BC1F-250D0F89AEDE}" name="Price"/>
-    <tableColumn id="4" xr3:uid="{AAC7EB66-2622-433B-B709-F1EA9DB2B157}" name="Quantity" totalsRowFunction="custom" dataDxfId="1" totalsRowDxfId="0">
+    <tableColumn id="4" xr3:uid="{AAC7EB66-2622-433B-B709-F1EA9DB2B157}" name="Quantity" totalsRowFunction="custom" dataDxfId="5" totalsRowDxfId="4">
       <totalsRowFormula>SUBTOTAL(109,D3:D14)</totalsRowFormula>
     </tableColumn>
   </tableColumns>
@@ -988,21 +1243,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC221F00-3B93-472A-A86B-EAEB3649F72B}">
-  <dimension ref="A2:I15"/>
+  <dimension ref="A2:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="4" width="10.1796875" customWidth="1"/>
-    <col min="8" max="8" width="12.36328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.54296875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="4" width="10.21875" customWidth="1"/>
+    <col min="8" max="8" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -1018,14 +1273,17 @@
       <c r="F2" t="s">
         <v>36</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="2" t="s">
         <v>32</v>
       </c>
       <c r="I2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -1035,21 +1293,24 @@
       <c r="C3">
         <v>10</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3">
         <v>2</v>
       </c>
       <c r="F3">
         <f>SUMPRODUCT(tblSales[Price],tblSales[Quantity])</f>
         <v>420</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="1">
+      <c r="I3" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J3" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -1059,17 +1320,20 @@
       <c r="C4">
         <v>10</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4">
         <v>2</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="H4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="I4" s="1">
+      <c r="I4" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J4" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -1079,17 +1343,20 @@
       <c r="C5">
         <v>10</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5">
         <v>2</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="H5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="1">
+      <c r="I5" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J5" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -1099,17 +1366,20 @@
       <c r="C6">
         <v>10</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6">
         <v>2</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="H6" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I6" s="1">
+      <c r="I6" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J6" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -1119,17 +1389,20 @@
       <c r="C7">
         <v>10</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7">
         <v>2</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="H7" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="I7" s="1">
+      <c r="I7" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J7" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -1139,17 +1412,20 @@
       <c r="C8">
         <v>10</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8">
         <v>2</v>
       </c>
-      <c r="H8" s="4" t="s">
+      <c r="H8" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="I8" s="1">
+      <c r="I8" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J8" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -1159,17 +1435,20 @@
       <c r="C9">
         <v>10</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9">
         <v>5</v>
       </c>
-      <c r="H9" s="4" t="s">
+      <c r="H9" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="I9" s="1">
+      <c r="I9" s="6">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J9" s="6">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -1179,17 +1458,20 @@
       <c r="C10">
         <v>10</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10">
         <v>5</v>
       </c>
-      <c r="H10" s="4" t="s">
+      <c r="H10" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="I10" s="1">
+      <c r="I10" s="6">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J10" s="6">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -1199,17 +1481,20 @@
       <c r="C11">
         <v>10</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11">
         <v>5</v>
       </c>
-      <c r="H11" s="4" t="s">
+      <c r="H11" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="I11" s="1">
+      <c r="I11" s="6">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J11" s="6">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -1219,17 +1504,20 @@
       <c r="C12">
         <v>10</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12">
         <v>5</v>
       </c>
-      <c r="H12" s="4" t="s">
+      <c r="H12" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="I12" s="1">
+      <c r="I12" s="6">
         <v>5</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J12" s="6">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -1239,17 +1527,20 @@
       <c r="C13">
         <v>10</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13">
         <v>5</v>
       </c>
-      <c r="H13" s="4" t="s">
+      <c r="H13" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="I13" s="1">
+      <c r="I13" s="6">
         <v>5</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J13" s="6">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -1259,30 +1550,36 @@
       <c r="C14">
         <v>10</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D14">
         <v>5</v>
       </c>
-      <c r="H14" s="4" t="s">
+      <c r="H14" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="I14" s="1">
+      <c r="I14" s="6">
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="D15" s="1">
-        <f t="shared" ref="C15:D15" si="0">SUBTOTAL(109,D3:D14)</f>
+      <c r="J14" s="6">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D15">
+        <f t="shared" ref="D15" si="0">SUBTOTAL(109,D3:D14)</f>
         <v>42</v>
       </c>
-      <c r="F15" s="5">
+      <c r="F15" s="4">
         <f>tblSales[[#Totals],[Price]]*tblSales[[#Totals],[Quantity]]</f>
         <v>0</v>
       </c>
-      <c r="H15" s="4" t="s">
+      <c r="H15" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="I15" s="1">
+      <c r="I15" s="6">
         <v>42</v>
+      </c>
+      <c r="J15" s="6">
+        <v>5040</v>
       </c>
     </row>
   </sheetData>
@@ -1301,18 +1598,18 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="11.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A4" s="1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4">
         <v>669463</v>
       </c>
     </row>
@@ -1324,18 +1621,22 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{077F63E6-078A-45B9-9241-E8D08A5A7DA9}">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="3" width="13" customWidth="1"/>
+    <col min="6" max="6" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -1345,243 +1646,338 @@
       <c r="C1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="1">
         <v>54383</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="5">
+        <v>151159</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="1">
         <v>44027</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="5">
+        <v>205658</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="1">
         <v>47664</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="5">
+        <v>312646</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>9</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="1">
         <v>31100</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F5" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" s="5">
+        <v>669463</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>10</v>
       </c>
       <c r="B6" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="1">
         <v>59112</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>11</v>
       </c>
       <c r="B7" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="1">
         <v>46124</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>12</v>
       </c>
       <c r="B8" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="1">
         <v>30236</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>6</v>
       </c>
       <c r="B9" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="1">
         <v>44318</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>7</v>
       </c>
       <c r="B10" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="1">
         <v>10384</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>8</v>
       </c>
       <c r="B11" t="s">
         <v>0</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="1">
         <v>17566</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>9</v>
       </c>
       <c r="B12" t="s">
         <v>0</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="1">
         <v>2568</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>10</v>
       </c>
       <c r="B13" t="s">
         <v>0</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="1">
         <v>27620</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>11</v>
       </c>
       <c r="B14" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="1">
         <v>24819</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>12</v>
       </c>
       <c r="B15" t="s">
         <v>0</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="1">
         <v>23884</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F15" t="s">
+        <v>6</v>
+      </c>
+      <c r="G15" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>6</v>
       </c>
       <c r="B16" t="s">
         <v>4</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="1">
         <v>22363</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F16" t="s">
+        <v>7</v>
+      </c>
+      <c r="G16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>7</v>
       </c>
       <c r="B17" t="s">
         <v>4</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="1">
         <v>5357</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F17" t="s">
+        <v>8</v>
+      </c>
+      <c r="G17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>8</v>
       </c>
       <c r="B18" t="s">
         <v>4</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="1">
         <v>11473</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F18" t="s">
+        <v>9</v>
+      </c>
+      <c r="G18" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>9</v>
       </c>
       <c r="B19" t="s">
         <v>4</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19" s="1">
         <v>57507</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F19" t="s">
+        <v>10</v>
+      </c>
+      <c r="G19" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>10</v>
       </c>
       <c r="B20" t="s">
         <v>4</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C20" s="1">
         <v>40516</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F20" t="s">
+        <v>11</v>
+      </c>
+      <c r="G20" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>11</v>
       </c>
       <c r="B21" t="s">
         <v>4</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C21" s="1">
         <v>12075</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F21" t="s">
+        <v>12</v>
+      </c>
+      <c r="G21" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>12</v>
       </c>
       <c r="B22" t="s">
         <v>4</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22" s="1">
         <v>56367</v>
+      </c>
+      <c r="G22" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G23" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G24" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G25" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G26" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>